<commit_message>
them sua xoa Dieuchuyen xuat exel
</commit_message>
<xml_diff>
--- a/DowloadMauPhieuNhap.xlsx
+++ b/DowloadMauPhieuNhap.xlsx
@@ -55,7 +55,7 @@
     <t>PHIẾU NHẬP KHO</t>
   </si>
   <si>
-    <t>Ngày: 03/04/2023</t>
+    <t>Ngày: 09/04/2023</t>
   </si>
   <si>
     <t>Nhập tại kho: Kho TBDH môn Công Nghệ</t>
@@ -94,10 +94,10 @@
     <t>Thành tiền</t>
   </si>
   <si>
-    <t>Các bài hát dành cho thanh niên, học sinh phục vụ các chủ đề hoạt động của các tháng</t>
-  </si>
-  <si>
-    <t>Bộ</t>
+    <t>Tấm gương của những người thành đạt</t>
+  </si>
+  <si>
+    <t>Cái</t>
   </si>
   <si>
     <t>Cộng tiền</t>
@@ -660,7 +660,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="F9" sqref="F9"/>
@@ -849,85 +849,173 @@
         <v>21</v>
       </c>
       <c r="C13" s="23">
-        <v>1</v>
+        <v>1810</v>
       </c>
       <c r="D13" s="23" t="s">
         <v>22</v>
       </c>
       <c r="E13" s="23">
-        <v>2</v>
+        <v>2000</v>
       </c>
       <c r="F13" s="23">
-        <v>12345</v>
+        <v>3258000</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:10" customHeight="1" ht="16.8">
-      <c r="A14" s="9"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="F14" s="22">
-        <v>12345</v>
+    <row r="14" spans="1:10" customHeight="1" ht="21">
+      <c r="A14" s="23">
+        <v>2</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="23">
+        <v>8</v>
+      </c>
+      <c r="D14" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="23">
+        <v>2000</v>
+      </c>
+      <c r="F14" s="23">
+        <v>14400</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:10" customHeight="1" ht="21">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
+      <c r="A15" s="23">
+        <v>3</v>
+      </c>
+      <c r="B15" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="23">
+        <v>10</v>
+      </c>
+      <c r="D15" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" s="23">
+        <v>2000</v>
+      </c>
+      <c r="F15" s="23">
+        <v>18000</v>
+      </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:10" customHeight="1" ht="21">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="23">
+        <v>4</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="23">
+        <v>10</v>
+      </c>
+      <c r="D16" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16" s="23">
+        <v>2000</v>
+      </c>
+      <c r="F16" s="23">
+        <v>18000</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:10" customHeight="1" ht="21">
+      <c r="A17" s="23">
+        <v>5</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="23">
+        <v>2</v>
+      </c>
+      <c r="D17" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="23">
+        <v>2000</v>
+      </c>
+      <c r="F17" s="23">
+        <v>3600</v>
+      </c>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+    </row>
+    <row r="18" spans="1:10" customHeight="1" ht="16.8">
+      <c r="A18" s="9"/>
+      <c r="B18" s="10"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F18" s="22">
+        <v>3312000</v>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+    </row>
+    <row r="19" spans="1:10" customHeight="1" ht="21">
+      <c r="A19" s="4"/>
+      <c r="B19" s="4"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+    </row>
+    <row r="20" spans="1:10" customHeight="1" ht="21">
+      <c r="A20" s="12" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:10" customHeight="1" ht="21">
-      <c r="B17" s="4" t="s">
+    <row r="21" spans="1:10" customHeight="1" ht="21">
+      <c r="B21" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E17" s="19" t="s">
+      <c r="E21" s="19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:10" customHeight="1" ht="21">
-      <c r="A18" s="24" t="s">
+    <row r="22" spans="1:10" customHeight="1" ht="21">
+      <c r="A22" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="24"/>
-      <c r="F18" s="24"/>
-    </row>
-    <row r="19" spans="1:10" customHeight="1" ht="21">
-      <c r="A19" s="25" t="s">
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="24"/>
+      <c r="F22" s="24"/>
+    </row>
+    <row r="23" spans="1:10" customHeight="1" ht="21">
+      <c r="A23" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="B19" s="25"/>
-      <c r="C19" s="25"/>
-      <c r="D19" s="25"/>
-      <c r="E19" s="25"/>
-      <c r="F19" s="25"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="16"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="25"/>
+      <c r="D23" s="25"/>
+      <c r="E23" s="25"/>
+      <c r="F23" s="25"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="16"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A22:F22"/>
+    <mergeCell ref="A23:F23"/>
     <mergeCell ref="A5:F5"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="A1:B1"/>

</xml_diff>

<commit_message>
cap nhat bao mat, bao hong
</commit_message>
<xml_diff>
--- a/DowloadMauPhieuNhap.xlsx
+++ b/DowloadMauPhieuNhap.xlsx
@@ -55,7 +55,7 @@
     <t>PHIẾU NHẬP KHO</t>
   </si>
   <si>
-    <t>Ngày: 09/04/2023</t>
+    <t>Ngày: 16/04/2023</t>
   </si>
   <si>
     <t>Nhập tại kho: Kho TBDH môn Công Nghệ</t>
@@ -660,7 +660,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="F9" sqref="F9"/>
@@ -849,7 +849,7 @@
         <v>21</v>
       </c>
       <c r="C13" s="23">
-        <v>1810</v>
+        <v>1808</v>
       </c>
       <c r="D13" s="23" t="s">
         <v>22</v>
@@ -858,7 +858,7 @@
         <v>2000</v>
       </c>
       <c r="F13" s="23">
-        <v>3258000</v>
+        <v>3254400</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
@@ -871,7 +871,7 @@
         <v>21</v>
       </c>
       <c r="C14" s="23">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D14" s="23" t="s">
         <v>22</v>
@@ -880,142 +880,76 @@
         <v>2000</v>
       </c>
       <c r="F14" s="23">
-        <v>14400</v>
+        <v>3600</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:10" customHeight="1" ht="21">
-      <c r="A15" s="23">
-        <v>3</v>
-      </c>
-      <c r="B15" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C15" s="23">
-        <v>10</v>
-      </c>
-      <c r="D15" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="23">
-        <v>2000</v>
-      </c>
-      <c r="F15" s="23">
-        <v>18000</v>
+    <row r="15" spans="1:10" customHeight="1" ht="16.8">
+      <c r="A15" s="9"/>
+      <c r="B15" s="10"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="10"/>
+      <c r="E15" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="22">
+        <v>3258000</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:10" customHeight="1" ht="21">
-      <c r="A16" s="23">
-        <v>4</v>
-      </c>
-      <c r="B16" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="23">
-        <v>10</v>
-      </c>
-      <c r="D16" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="23">
-        <v>2000</v>
-      </c>
-      <c r="F16" s="23">
-        <v>18000</v>
-      </c>
+      <c r="A16" s="4"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:10" customHeight="1" ht="21">
-      <c r="A17" s="23">
-        <v>5</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>21</v>
-      </c>
-      <c r="C17" s="23">
-        <v>2</v>
-      </c>
-      <c r="D17" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="E17" s="23">
-        <v>2000</v>
-      </c>
-      <c r="F17" s="23">
-        <v>3600</v>
-      </c>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="1:10" customHeight="1" ht="16.8">
-      <c r="A18" s="9"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="21" t="s">
-        <v>23</v>
-      </c>
-      <c r="F18" s="22">
-        <v>3312000</v>
-      </c>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
+      <c r="A17" s="12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" customHeight="1" ht="21">
+      <c r="B18" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="19" spans="1:10" customHeight="1" ht="21">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
+      <c r="A19" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
+      <c r="D19" s="24"/>
+      <c r="E19" s="24"/>
+      <c r="F19" s="24"/>
     </row>
     <row r="20" spans="1:10" customHeight="1" ht="21">
-      <c r="A20" s="12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" customHeight="1" ht="21">
-      <c r="B21" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E21" s="19" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" customHeight="1" ht="21">
-      <c r="A22" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" s="24"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="24"/>
-      <c r="F22" s="24"/>
-    </row>
-    <row r="23" spans="1:10" customHeight="1" ht="21">
-      <c r="A23" s="25" t="s">
+      <c r="A20" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="B23" s="25"/>
-      <c r="C23" s="25"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="25"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="16"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="25"/>
+      <c r="D20" s="25"/>
+      <c r="E20" s="25"/>
+      <c r="F20" s="25"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="16"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
-    <mergeCell ref="A22:F22"/>
-    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="A19:F19"/>
+    <mergeCell ref="A20:F20"/>
     <mergeCell ref="A5:F5"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="A1:B1"/>

</xml_diff>